<commit_message>
CR for code change
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,28 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55646C\Documents\UiPath\P003_090_TimesheetApprovals\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55646C\Documents\GitHub\P003_090_TimesheetApprovals_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{537C3E8A-D2FE-44CA-B4DB-C4067FBB835A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB47244-8AAF-48EE-903E-8467F84E2436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
     <sheet name="Constants" sheetId="2" r:id="rId2"/>
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="117">
   <si>
     <t>Name</t>
   </si>
@@ -155,63 +168,27 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>RPT00169_API_Url</t>
-  </si>
-  <si>
-    <t>169ResponseKey</t>
-  </si>
-  <si>
-    <t>169ReportPath</t>
-  </si>
-  <si>
     <t>169ReportSheetName</t>
   </si>
   <si>
-    <t>Report_Entry</t>
-  </si>
-  <si>
     <t>RPT00169</t>
   </si>
   <si>
     <t>OrchestratorQueueName</t>
   </si>
   <si>
-    <t>RPT00177_API_Url</t>
-  </si>
-  <si>
-    <t>177ResponseKey</t>
-  </si>
-  <si>
-    <t>177ReportPath</t>
-  </si>
-  <si>
     <t>177ReportSheetName</t>
   </si>
   <si>
     <t>RPT00177</t>
   </si>
   <si>
-    <t>KillApplications</t>
-  </si>
-  <si>
-    <t>Excel</t>
-  </si>
-  <si>
-    <t>Give all applications ; separated</t>
-  </si>
-  <si>
     <t>P003_090_TimesheetApprovals_RPT00169APICredential</t>
   </si>
   <si>
     <t>P003_090_TimesheetApprovals_RPT00177APICredential</t>
   </si>
   <si>
-    <t>DEV</t>
-  </si>
-  <si>
-    <t>TestRun</t>
-  </si>
-  <si>
     <t>O365TenantIDAssetName</t>
   </si>
   <si>
@@ -242,24 +219,12 @@
     <t>ExceptionMailSubject</t>
   </si>
   <si>
-    <t>Action Required: P003_090_TimesheetApprovals - Dispatcher Failed</t>
-  </si>
-  <si>
-    <t>ExceptionMailBody</t>
-  </si>
-  <si>
     <t>O365AssetsInOrchestratorFolder</t>
   </si>
   <si>
     <t>P003_090_TimesheetApprovals_Queue</t>
   </si>
   <si>
-    <t>Sharepoint URL</t>
-  </si>
-  <si>
-    <t>Root Folder</t>
-  </si>
-  <si>
     <t>177ReportName</t>
   </si>
   <si>
@@ -272,29 +237,164 @@
     <t>RPT00177 - {datetime}.xlsx</t>
   </si>
   <si>
-    <t>Data\Output\</t>
-  </si>
-  <si>
-    <t>Hello RPA Support Team,&lt;br&gt;&lt;br&gt;This email notification was raised for process P003_090_TimesheetApprovals_Dispatcher. The process execution met a System exception, details for which can be found below:&lt;br&gt;&lt;br&gt;&lt;b&gt;Exception:&lt;/b&gt; {exmsg}&lt;/b&gt;&lt;br&gt;&lt;br&gt;Regards,&lt;br&gt;P003_090_TimesheetApprovals bot.</t>
+    <t>SE_SPUnavailable</t>
+  </si>
+  <si>
+    <t>SE_RPT00177WorkdayAPI Unavailable</t>
+  </si>
+  <si>
+    <t>SE_RPT00169WorkdayAPI Unavailable</t>
+  </si>
+  <si>
+    <t>TimeoutMS</t>
+  </si>
+  <si>
+    <t>NoOfRetry</t>
+  </si>
+  <si>
+    <t>RetryInterval</t>
+  </si>
+  <si>
+    <t>SharepointInputFolderName</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>00:00:05</t>
+  </si>
+  <si>
+    <t>P003_090_TimesheetApprovals_RPT00169URL</t>
+  </si>
+  <si>
+    <t>P003_090_TimesheetApprovals_RPT00177URL</t>
+  </si>
+  <si>
+    <t>P003_090_TimesheetApprovals_SPURL</t>
+  </si>
+  <si>
+    <t>P003_090_TimesheetApprovals_SPRootFolder</t>
+  </si>
+  <si>
+    <t>ProcessFolderName</t>
+  </si>
+  <si>
+    <t>CreateLocalFolderWorkflowSE</t>
+  </si>
+  <si>
+    <t>Bot was not able to create the local folder.</t>
+  </si>
+  <si>
+    <t>P003_090_TimesheetApprovals_LocalRootFolder</t>
+  </si>
+  <si>
+    <t>LocalFolderNotPresentSE</t>
+  </si>
+  <si>
+    <t>Local folder is not exists.</t>
+  </si>
+  <si>
+    <t>LocalFolderPath</t>
+  </si>
+  <si>
+    <t>Subject_RPT00177WorkdayAPI Unavailable</t>
+  </si>
+  <si>
+    <t>System Exception - Unable to download RPT00177 from the Workday API</t>
+  </si>
+  <si>
+    <t>System Exception - Unable to download RPT00169 from the Workday API</t>
+  </si>
+  <si>
+    <t>strSubject</t>
+  </si>
+  <si>
+    <t>Subject_RPT00169WorkdayAPI Unavailable</t>
+  </si>
+  <si>
+    <t>Subject_SharepointUnavailable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Exception - Unable to Access Bot Sharepoint </t>
+  </si>
+  <si>
+    <t>connectivity issue for sharepoint.</t>
+  </si>
+  <si>
+    <t>BotAutomationFolder</t>
+  </si>
+  <si>
+    <t>BotWorkingFolder</t>
+  </si>
+  <si>
+    <t>Automation</t>
+  </si>
+  <si>
+    <t>TimesheetApprovals</t>
+  </si>
+  <si>
+    <t>Exception - Timesheet Entry Approval Process Failed</t>
   </si>
   <si>
     <t>P003_090_TimesheetApprovals</t>
   </si>
   <si>
-    <t>https://wd2-impl-services1.workday.com/ccx/service/customreport2/okgov/Jerry.Schnellbacher%40omes.ok.gov/RPT00169_-_Reported_Time_Not_Approved_RAAS</t>
-  </si>
-  <si>
-    <t>https://wd2-impl-services1.workday.com/ccx/service/customreport2/okgov/ISU_RPT00177/Rpt00177_-_No_Time_Reported_Between_Dates_RAAS</t>
-  </si>
-  <si>
-    <t>https://officemgmtentserv.sharepoint.com/sites/ACOE_Automations</t>
+    <t>SharepointFolderCreationSE</t>
+  </si>
+  <si>
+    <t>Sharepoint folder creatio flow has system exception</t>
+  </si>
+  <si>
+    <t>GetLastWeekDatesSE</t>
+  </si>
+  <si>
+    <t>Get Last week dates flow has system exception</t>
+  </si>
+  <si>
+    <t>Convert JsonToExcelSE</t>
+  </si>
+  <si>
+    <t>Json to Excel convertion flow has system exception</t>
+  </si>
+  <si>
+    <t>P003_090_TimesheetApprovals_ExceptionMailBody</t>
+  </si>
+  <si>
+    <t>P003_090_TimesheetApprovals_169ResponseKey</t>
+  </si>
+  <si>
+    <t>P003_090_TimesheetApprovals_177ResponseKey</t>
+  </si>
+  <si>
+    <t>issue in Workday RPT00177 API</t>
+  </si>
+  <si>
+    <t>issue in Workday RPT00169 API</t>
+  </si>
+  <si>
+    <t>Subject_WorkdayAPI Unavailable</t>
+  </si>
+  <si>
+    <t>System Exception - Unable to download RPT00177 &amp;  RPT00169 from the Workday API</t>
+  </si>
+  <si>
+    <t>BotEnvironmentFolder</t>
+  </si>
+  <si>
+    <t>CF_-_Awaiting_Persons_Emails_PT</t>
+  </si>
+  <si>
+    <t>Awaiting_Persons_Emails</t>
+  </si>
+  <si>
+    <t>PROD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -330,18 +430,6 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF323130"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -360,11 +448,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -376,13 +463,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -695,10 +778,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z995"/>
+  <dimension ref="A1:Z977"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -745,10 +828,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
@@ -758,8 +841,9 @@
       <c r="A3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>60</v>
+      <c r="B3" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!B2,"/P003_090_TimesheetApprovals")</f>
+        <v>PROD/P003_090_TimesheetApprovals</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>31</v>
@@ -781,192 +865,261 @@
       <c r="C6" s="4"/>
     </row>
     <row r="7" spans="1:26">
-      <c r="A7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26">
-      <c r="C8" s="4"/>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+        <v>63</v>
+      </c>
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>85</v>
+      <c r="A11" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A12" t="s">
-        <v>44</v>
+      <c r="A12" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="B13" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B15" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
+        <v>60</v>
+      </c>
+      <c r="B15" t="str">
+        <f>Constants!B2</f>
+        <v>PROD</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:2" ht="14.25" customHeight="1">
       <c r="A17" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B17" t="s">
-        <v>47</v>
+        <v>59</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1">
       <c r="A18" s="2" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1">
       <c r="A19" s="2" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>54</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1">
       <c r="A20" s="2" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>81</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1">
       <c r="A21" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B21" t="s">
-        <v>63</v>
+        <v>69</v>
+      </c>
+      <c r="B21">
+        <v>100000</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B22" t="s">
-        <v>64</v>
+        <v>70</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="14.25" customHeight="1">
       <c r="A23" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B23" t="s">
-        <v>66</v>
+        <v>71</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="14.25" customHeight="1">
       <c r="A24" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B24" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A25" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B25" t="s">
+        <v>97</v>
+      </c>
+    </row>
     <row r="26" spans="1:2" ht="14.25" customHeight="1">
       <c r="A26" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>72</v>
+        <v>80</v>
+      </c>
+      <c r="B26" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="14.25" customHeight="1">
       <c r="A27" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B27" s="2" t="s">
         <v>83</v>
+      </c>
+      <c r="B27" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="14.25" customHeight="1">
       <c r="A28" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="14.25" customHeight="1">
       <c r="A29" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
+        <v>86</v>
+      </c>
+      <c r="B29" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A30" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B30" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A31" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A32" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B32" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A33" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B33" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A34" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B34" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A35" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B35" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A36" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A37" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B37" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A38" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B38" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A39" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="41" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="42" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="43" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="44" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="45" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="46" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="47" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="48" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>
@@ -1896,42 +2049,19 @@
     <row r="975" ht="14.25" customHeight="1"/>
     <row r="976" ht="14.25" customHeight="1"/>
     <row r="977" ht="14.25" customHeight="1"/>
-    <row r="978" ht="14.25" customHeight="1"/>
-    <row r="979" ht="14.25" customHeight="1"/>
-    <row r="980" ht="14.25" customHeight="1"/>
-    <row r="981" ht="14.25" customHeight="1"/>
-    <row r="982" ht="14.25" customHeight="1"/>
-    <row r="983" ht="14.25" customHeight="1"/>
-    <row r="984" ht="14.25" customHeight="1"/>
-    <row r="985" ht="14.25" customHeight="1"/>
-    <row r="986" ht="14.25" customHeight="1"/>
-    <row r="987" ht="14.25" customHeight="1"/>
-    <row r="988" ht="14.25" customHeight="1"/>
-    <row r="989" ht="14.25" customHeight="1"/>
-    <row r="990" ht="14.25" customHeight="1"/>
-    <row r="991" ht="14.25" customHeight="1"/>
-    <row r="992" ht="14.25" customHeight="1"/>
-    <row r="993" ht="14.25" customHeight="1"/>
-    <row r="994" ht="14.25" customHeight="1"/>
-    <row r="995" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
-  <hyperlinks>
-    <hyperlink ref="B11" r:id="rId1" xr:uid="{0F30253A-7998-4331-AF6D-CE2C1DC2203B}"/>
-    <hyperlink ref="B16" r:id="rId2" xr:uid="{1DD869C7-DE09-4321-AFA7-73D42D6FA82E}"/>
-    <hyperlink ref="B28" r:id="rId3" xr:uid="{16D98946-5C94-4A7D-9FD8-76EEE4742974}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z988"/>
+  <dimension ref="A1:Z989"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1976,143 +2106,174 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+    </row>
+    <row r="3" spans="1:26" ht="30">
+      <c r="A3" t="s">
         <v>5</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" ht="45">
-      <c r="A3" t="s">
-        <v>32</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="45">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A5" t="s">
+    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>28</v>
-      </c>
-    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
         <v>33</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>42</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A14" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14">
-        <v>2</v>
-      </c>
-      <c r="C14" t="s">
-        <v>37</v>
-      </c>
-    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="45">
-      <c r="A17" t="s">
+    <row r="17" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="18" spans="1:3" ht="45">
+      <c r="A18" t="s">
         <v>39</v>
       </c>
-      <c r="B17" t="b">
+      <c r="B18" t="b">
         <v>0</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
@@ -3083,6 +3244,7 @@
     <row r="986" ht="14.25" customHeight="1"/>
     <row r="987" ht="14.25" customHeight="1"/>
     <row r="988" ht="14.25" customHeight="1"/>
+    <row r="989" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3094,12 +3256,12 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="1" max="1" width="53.42578125" customWidth="1"/>
     <col min="2" max="2" width="30.140625" customWidth="1"/>
     <col min="3" max="3" width="60.28515625" customWidth="1"/>
     <col min="4" max="26" width="65.42578125" customWidth="1"/>
@@ -3143,67 +3305,160 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C2" t="s">
-        <v>60</v>
+        <v>48</v>
+      </c>
+      <c r="C2" t="str">
+        <f>_xlfn.CONCAT(Constants!B2,"/P003_090_TimesheetApprovals")</f>
+        <v>PROD/P003_090_TimesheetApprovals</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" t="s">
-        <v>60</v>
+        <v>49</v>
+      </c>
+      <c r="C3" t="str">
+        <f>_xlfn.CONCAT(Constants!B2,"/P003_090_TimesheetApprovals")</f>
+        <v>PROD/P003_090_TimesheetApprovals</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C4" t="s">
-        <v>60</v>
+        <v>56</v>
+      </c>
+      <c r="C4" t="str">
+        <f>_xlfn.CONCAT(Constants!B2,"/P003_090_TimesheetApprovals")</f>
+        <v>PROD/P003_090_TimesheetApprovals</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" s="6" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C5" t="s">
-        <v>60</v>
+        <v>57</v>
+      </c>
+      <c r="C5" t="str">
+        <f>_xlfn.CONCAT(Constants!B2,"/P003_090_TimesheetApprovals")</f>
+        <v>PROD/P003_090_TimesheetApprovals</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+        <v>58</v>
+      </c>
+      <c r="C6" t="str">
+        <f>_xlfn.CONCAT(Constants!B2,"/P003_090_TimesheetApprovals")</f>
+        <v>PROD/P003_090_TimesheetApprovals</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" t="str">
+        <f>_xlfn.CONCAT(Constants!B2,"/P003_090_TimesheetApprovals")</f>
+        <v>PROD/P003_090_TimesheetApprovals</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" t="str">
+        <f>_xlfn.CONCAT(Constants!B2,"/P003_090_TimesheetApprovals")</f>
+        <v>PROD/P003_090_TimesheetApprovals</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" t="str">
+        <f>_xlfn.CONCAT(Constants!B2,"/P003_090_TimesheetApprovals")</f>
+        <v>PROD/P003_090_TimesheetApprovals</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" t="str">
+        <f>_xlfn.CONCAT(Constants!B2,"/P003_090_TimesheetApprovals")</f>
+        <v>PROD/P003_090_TimesheetApprovals</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" t="str">
+        <f>_xlfn.CONCAT(Constants!B2,"/P003_090_TimesheetApprovals")</f>
+        <v>PROD/P003_090_TimesheetApprovals</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>106</v>
+      </c>
+      <c r="B12" t="s">
+        <v>106</v>
+      </c>
+      <c r="C12" t="str">
+        <f>_xlfn.CONCAT(Constants!B2,"/P003_090_TimesheetApprovals")</f>
+        <v>PROD/P003_090_TimesheetApprovals</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>107</v>
+      </c>
+      <c r="B13" t="s">
+        <v>107</v>
+      </c>
+      <c r="C13" t="str">
+        <f>_xlfn.CONCAT(Constants!B2,"/P003_090_TimesheetApprovals")</f>
+        <v>PROD/P003_090_TimesheetApprovals</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C14" t="str">
+        <f>_xlfn.CONCAT(Constants!B2,"/P003_090_TimesheetApprovals")</f>
+        <v>PROD/P003_090_TimesheetApprovals</v>
+      </c>
+    </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
kill process added for current user
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55646C\Documents\GitHub\P003_090_TimesheetApprovals_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB47244-8AAF-48EE-903E-8467F84E2436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{549A5E08-B008-4176-B32B-D40E9289EA13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -781,7 +781,7 @@
   <dimension ref="A1:Z977"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2061,7 +2061,7 @@
   <dimension ref="A1:Z989"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
updates to allow multiple agencies
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55646C\Documents\GitHub\P003_090_TimesheetApprovals_Dispatcher\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\57145C\Documents\UiPath\P003_090_TimesheetApprovals_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{549A5E08-B008-4176-B32B-D40E9289EA13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77DA358C-6F54-4E30-A98C-B918FE26CAB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="9360" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="124">
   <si>
     <t>Name</t>
   </si>
@@ -388,6 +388,27 @@
   </si>
   <si>
     <t>PROD</t>
+  </si>
+  <si>
+    <t>P003_090_TimesheetApprovals_AgencyReferenceFile</t>
+  </si>
+  <si>
+    <t>AgencyReferenceFile</t>
+  </si>
+  <si>
+    <t>AgencyRef.xlsx</t>
+  </si>
+  <si>
+    <t>P003_090_TimesheetApprovals_RPT00177URLv2</t>
+  </si>
+  <si>
+    <t>P003_090_TimesheetApprovals_RPT00169URLv2</t>
+  </si>
+  <si>
+    <t>P003_090_TimesheetApprovals_RPT00177APICredentialv2</t>
+  </si>
+  <si>
+    <t>P003_090_TimesheetApprovals_RPT00169APICredentialv2</t>
   </si>
 </sst>
 </file>
@@ -778,18 +799,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z977"/>
+  <dimension ref="A1:Z976"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
-    <col min="2" max="2" width="232.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" customWidth="1"/>
+    <col min="2" max="2" width="232.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -828,29 +849,29 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" ht="45">
-      <c r="A3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="2" t="str">
+      <c r="B2" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P003_090_TimesheetApprovals")</f>
         <v>PROD/P003_090_TimesheetApprovals</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>31</v>
       </c>
     </row>
+    <row r="3" spans="1:26" ht="14.5">
+      <c r="A3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="30">
+    <row r="5" spans="1:26" ht="29">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -861,10 +882,10 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:26" ht="14.5">
       <c r="C6" s="4"/>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:26" ht="14.5">
       <c r="C7" s="4"/>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1111,7 +1132,14 @@
         <v>114</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="40" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A40" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
     <row r="41" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="42" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="43" spans="1:2" ht="14.25" customHeight="1"/>
@@ -2048,8 +2076,10 @@
     <row r="974" ht="14.25" customHeight="1"/>
     <row r="975" ht="14.25" customHeight="1"/>
     <row r="976" ht="14.25" customHeight="1"/>
-    <row r="977" ht="14.25" customHeight="1"/>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C3">
+    <sortCondition ref="A1:A3"/>
+  </sortState>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2060,16 +2090,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z989"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2138,7 +2168,7 @@
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
-    <row r="3" spans="1:26" ht="30">
+    <row r="3" spans="1:26" ht="29">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -2149,7 +2179,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="45">
+    <row r="4" spans="1:26" ht="43.5">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -2263,7 +2293,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="18" spans="1:3" ht="45">
+    <row r="18" spans="1:3" ht="29">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -3255,16 +3285,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="53.42578125" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="51.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -3308,10 +3338,10 @@
         <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>123</v>
       </c>
       <c r="C2" t="str">
-        <f>_xlfn.CONCAT(Constants!B2,"/P003_090_TimesheetApprovals")</f>
+        <f>_xlfn.CONCAT(Constants!$B$2,"/P003_090_TimesheetApprovals")</f>
         <v>PROD/P003_090_TimesheetApprovals</v>
       </c>
     </row>
@@ -3320,10 +3350,10 @@
         <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>122</v>
       </c>
       <c r="C3" t="str">
-        <f>_xlfn.CONCAT(Constants!B2,"/P003_090_TimesheetApprovals")</f>
+        <f>_xlfn.CONCAT(Constants!$B$2,"/P003_090_TimesheetApprovals")</f>
         <v>PROD/P003_090_TimesheetApprovals</v>
       </c>
     </row>
@@ -3335,7 +3365,7 @@
         <v>56</v>
       </c>
       <c r="C4" t="str">
-        <f>_xlfn.CONCAT(Constants!B2,"/P003_090_TimesheetApprovals")</f>
+        <f>_xlfn.CONCAT(Constants!$B$2,"/P003_090_TimesheetApprovals")</f>
         <v>PROD/P003_090_TimesheetApprovals</v>
       </c>
     </row>
@@ -3347,7 +3377,7 @@
         <v>57</v>
       </c>
       <c r="C5" t="str">
-        <f>_xlfn.CONCAT(Constants!B2,"/P003_090_TimesheetApprovals")</f>
+        <f>_xlfn.CONCAT(Constants!$B$2,"/P003_090_TimesheetApprovals")</f>
         <v>PROD/P003_090_TimesheetApprovals</v>
       </c>
     </row>
@@ -3359,7 +3389,7 @@
         <v>58</v>
       </c>
       <c r="C6" t="str">
-        <f>_xlfn.CONCAT(Constants!B2,"/P003_090_TimesheetApprovals")</f>
+        <f>_xlfn.CONCAT(Constants!$B$2,"/P003_090_TimesheetApprovals")</f>
         <v>PROD/P003_090_TimesheetApprovals</v>
       </c>
     </row>
@@ -3368,10 +3398,10 @@
         <v>75</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>121</v>
       </c>
       <c r="C7" t="str">
-        <f>_xlfn.CONCAT(Constants!B2,"/P003_090_TimesheetApprovals")</f>
+        <f>_xlfn.CONCAT(Constants!$B$2,"/P003_090_TimesheetApprovals")</f>
         <v>PROD/P003_090_TimesheetApprovals</v>
       </c>
     </row>
@@ -3380,10 +3410,10 @@
         <v>76</v>
       </c>
       <c r="B8" t="s">
-        <v>76</v>
+        <v>120</v>
       </c>
       <c r="C8" t="str">
-        <f>_xlfn.CONCAT(Constants!B2,"/P003_090_TimesheetApprovals")</f>
+        <f>_xlfn.CONCAT(Constants!$B$2,"/P003_090_TimesheetApprovals")</f>
         <v>PROD/P003_090_TimesheetApprovals</v>
       </c>
     </row>
@@ -3395,7 +3425,7 @@
         <v>77</v>
       </c>
       <c r="C9" t="str">
-        <f>_xlfn.CONCAT(Constants!B2,"/P003_090_TimesheetApprovals")</f>
+        <f>_xlfn.CONCAT(Constants!$B$2,"/P003_090_TimesheetApprovals")</f>
         <v>PROD/P003_090_TimesheetApprovals</v>
       </c>
     </row>
@@ -3407,7 +3437,7 @@
         <v>78</v>
       </c>
       <c r="C10" t="str">
-        <f>_xlfn.CONCAT(Constants!B2,"/P003_090_TimesheetApprovals")</f>
+        <f>_xlfn.CONCAT(Constants!$B$2,"/P003_090_TimesheetApprovals")</f>
         <v>PROD/P003_090_TimesheetApprovals</v>
       </c>
     </row>
@@ -3419,7 +3449,7 @@
         <v>82</v>
       </c>
       <c r="C11" t="str">
-        <f>_xlfn.CONCAT(Constants!B2,"/P003_090_TimesheetApprovals")</f>
+        <f>_xlfn.CONCAT(Constants!$B$2,"/P003_090_TimesheetApprovals")</f>
         <v>PROD/P003_090_TimesheetApprovals</v>
       </c>
     </row>
@@ -3431,7 +3461,7 @@
         <v>106</v>
       </c>
       <c r="C12" t="str">
-        <f>_xlfn.CONCAT(Constants!B2,"/P003_090_TimesheetApprovals")</f>
+        <f>_xlfn.CONCAT(Constants!$B$2,"/P003_090_TimesheetApprovals")</f>
         <v>PROD/P003_090_TimesheetApprovals</v>
       </c>
     </row>
@@ -3443,7 +3473,7 @@
         <v>107</v>
       </c>
       <c r="C13" t="str">
-        <f>_xlfn.CONCAT(Constants!B2,"/P003_090_TimesheetApprovals")</f>
+        <f>_xlfn.CONCAT(Constants!$B$2,"/P003_090_TimesheetApprovals")</f>
         <v>PROD/P003_090_TimesheetApprovals</v>
       </c>
     </row>
@@ -3455,11 +3485,22 @@
         <v>108</v>
       </c>
       <c r="C14" t="str">
-        <f>_xlfn.CONCAT(Constants!B2,"/P003_090_TimesheetApprovals")</f>
+        <f>_xlfn.CONCAT(Constants!$B$2,"/P003_090_TimesheetApprovals")</f>
         <v>PROD/P003_090_TimesheetApprovals</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
+        <v>117</v>
+      </c>
+      <c r="B15" t="s">
+        <v>117</v>
+      </c>
+      <c r="C15" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$2,"/P003_090_TimesheetApprovals")</f>
+        <v>PROD/P003_090_TimesheetApprovals</v>
+      </c>
+    </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>

</xml_diff>